<commit_message>
result of greedy algorithms
</commit_message>
<xml_diff>
--- a/data/result_op_greedy_algo.xlsx
+++ b/data/result_op_greedy_algo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nightraven/Coding/optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C239C4-5104-F44F-B104-061BB1B416FF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB2A5A3-EDA2-9943-B3A9-5D2EB03886D6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="460" windowWidth="27640" windowHeight="15820" xr2:uid="{7DA1179F-BE88-A549-9FA8-FD417347C3A0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="69">
   <si>
     <t>mymodockerhqelk03</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>Move 2 vms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total vm in 4 servers </t>
+  </si>
+  <si>
+    <t>58 + 4(ovsapp)</t>
   </si>
 </sst>
 </file>
@@ -1004,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1E477B-084F-5A42-A515-512E8B19ED4B}">
   <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1837,6 +1843,12 @@
       </c>
     </row>
     <row r="28" spans="1:17">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
       <c r="G28" s="2" t="s">
         <v>31</v>
       </c>

</xml_diff>